<commit_message>
add capital benefit calculator for SO
</commit_message>
<xml_diff>
--- a/data/SO/Steuerfuesse_NP_2000-2019.xlsx
+++ b/data/SO/Steuerfuesse_NP_2000-2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\PensionTools\data\SO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20A42894-C2A4-455E-A95A-3BAD7FFC87FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7F82FB-DDEF-4B1D-8CD7-352B007D30A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -921,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>

</xml_diff>